<commit_message>
Add Solr search functionality and update library data
</commit_message>
<xml_diff>
--- a/library.xlsx
+++ b/library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\URA\URA-word-seperator\bahnar-word-split-and-example-finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D31BC0D-A5D1-4E81-ACDD-43EE2E12777F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BCE895-63B0-4116-AA78-1CC3C8859C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19710" yWindow="3285" windowWidth="15015" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B176"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A154" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>